<commit_message>
Update scrum and add justification doc
</commit_message>
<xml_diff>
--- a/Documents/burndown-1.xlsx
+++ b/Documents/burndown-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="105">
   <si>
     <t>Today</t>
   </si>
@@ -259,6 +259,11 @@
     <t>Dates</t>
   </si>
   <si>
+    <t>Done: Discussed game ideas
+Next: Nail down core mechanics
+Help: --</t>
+  </si>
+  <si>
     <t>Done: Threw around ideas for game
 Next: Finalized game's core mechanics
 Help: —</t>
@@ -279,9 +284,24 @@
 Help: —</t>
   </si>
   <si>
+    <t>Done: Implement basic block interactions
+Next: Clean up block logic
+Help: --</t>
+  </si>
+  <si>
     <t>Done: Rudimentary Player script
 Next: —
 Help: —</t>
+  </si>
+  <si>
+    <t>Done: Make block logic pretty, started on block separation logic
+Next: Finish block separations
+Help: --</t>
+  </si>
+  <si>
+    <t>Done: Finished block separations
+Next: --
+Help: --</t>
   </si>
   <si>
     <t>Done: Completed game research and planned out part of R and A 
@@ -318,6 +338,11 @@
 Help: —</t>
   </si>
   <si>
+    <t>Done: R&amp;A for 2 games
+Next: Add in phases and win conditions
+Help: --</t>
+  </si>
+  <si>
     <t xml:space="preserve">Done: Not much. Some stuff with block collision bug
 Next: Item spawners and object pooling prototype
 </t>
@@ -331,6 +356,11 @@
     <t>Done: 3 player controls
 Next: —
 Help: —</t>
+  </si>
+  <si>
+    <t>Done: Win conditions and phases
+Next: --
+Help: --</t>
   </si>
   <si>
     <t>Done: Block spawners and bugtesting, item placement guidance
@@ -1119,8 +1149,8 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="530291784"/>
-        <c:axId val="1014575596"/>
+        <c:axId val="651114837"/>
+        <c:axId val="372472017"/>
       </c:areaChart>
       <c:lineChart>
         <c:varyColors val="0"/>
@@ -1149,11 +1179,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="530291784"/>
-        <c:axId val="1014575596"/>
+        <c:axId val="651114837"/>
+        <c:axId val="372472017"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="530291784"/>
+        <c:axId val="651114837"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,10 +1215,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014575596"/>
+        <c:crossAx val="372472017"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1014575596"/>
+        <c:axId val="372472017"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,7 +1266,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530291784"/>
+        <c:crossAx val="651114837"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1520,8 +1550,8 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1476600606"/>
-        <c:axId val="2001978118"/>
+        <c:axId val="1669947738"/>
+        <c:axId val="869827041"/>
       </c:areaChart>
       <c:lineChart>
         <c:varyColors val="0"/>
@@ -1555,11 +1585,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1476600606"/>
-        <c:axId val="2001978118"/>
+        <c:axId val="1669947738"/>
+        <c:axId val="869827041"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1476600606"/>
+        <c:axId val="1669947738"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,10 +1621,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2001978118"/>
+        <c:crossAx val="869827041"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2001978118"/>
+        <c:axId val="869827041"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1672,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1476600606"/>
+        <c:crossAx val="1669947738"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -44036,10 +44066,12 @@
       </c>
       <c r="D8" s="86"/>
       <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
+      <c r="F8" s="85" t="s">
+        <v>81</v>
+      </c>
       <c r="G8" s="86"/>
       <c r="H8" s="85" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I8" s="86"/>
       <c r="J8" s="29"/>
@@ -44110,12 +44142,12 @@
       </c>
       <c r="D10" s="86"/>
       <c r="E10" s="85" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F10" s="86"/>
       <c r="G10" s="86"/>
       <c r="H10" s="85" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I10" s="86"/>
       <c r="J10" s="29"/>
@@ -44150,9 +44182,11 @@
       </c>
       <c r="D11" s="86"/>
       <c r="E11" s="85" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="86"/>
+        <v>85</v>
+      </c>
+      <c r="F11" s="85" t="s">
+        <v>86</v>
+      </c>
       <c r="G11" s="86"/>
       <c r="H11" s="86"/>
       <c r="I11" s="86"/>
@@ -44188,9 +44222,11 @@
       </c>
       <c r="D12" s="86"/>
       <c r="E12" s="85" t="s">
-        <v>85</v>
-      </c>
-      <c r="F12" s="86"/>
+        <v>87</v>
+      </c>
+      <c r="F12" s="85" t="s">
+        <v>88</v>
+      </c>
       <c r="G12" s="86"/>
       <c r="H12" s="86"/>
       <c r="I12" s="86"/>
@@ -44262,7 +44298,9 @@
       </c>
       <c r="D14" s="86"/>
       <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
+      <c r="F14" s="85" t="s">
+        <v>89</v>
+      </c>
       <c r="G14" s="86"/>
       <c r="H14" s="86"/>
       <c r="I14" s="86"/>
@@ -44300,7 +44338,7 @@
       <c r="E15" s="86"/>
       <c r="F15" s="86"/>
       <c r="G15" s="85" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H15" s="86"/>
       <c r="I15" s="86"/>
@@ -44335,7 +44373,7 @@
         <v>Tue</v>
       </c>
       <c r="D16" s="85" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E16" s="86"/>
       <c r="F16" s="86"/>
@@ -44373,7 +44411,7 @@
         <v>Wed</v>
       </c>
       <c r="D17" s="85" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E17" s="86"/>
       <c r="F17" s="86"/>
@@ -44411,12 +44449,12 @@
         <v>Thu</v>
       </c>
       <c r="D18" s="85" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E18" s="86"/>
       <c r="F18" s="86"/>
       <c r="G18" s="85" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H18" s="86"/>
       <c r="I18" s="86"/>
@@ -44451,7 +44489,7 @@
         <v>Fri</v>
       </c>
       <c r="D19" s="85" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E19" s="86"/>
       <c r="F19" s="86"/>
@@ -44490,11 +44528,13 @@
       </c>
       <c r="D20" s="86"/>
       <c r="E20" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="86"/>
+        <v>96</v>
+      </c>
+      <c r="F20" s="85" t="s">
+        <v>97</v>
+      </c>
       <c r="G20" s="85" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="H20" s="86"/>
       <c r="I20" s="86"/>
@@ -44529,17 +44569,19 @@
         <v>Sun</v>
       </c>
       <c r="D21" s="85" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E21" s="85" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="86"/>
+        <v>100</v>
+      </c>
+      <c r="F21" s="85" t="s">
+        <v>101</v>
+      </c>
       <c r="G21" s="85" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="H21" s="85" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="I21" s="86"/>
       <c r="J21" s="29"/>
@@ -44576,7 +44618,7 @@
       <c r="E22" s="86"/>
       <c r="F22" s="86"/>
       <c r="G22" s="85" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="H22" s="86"/>
       <c r="I22" s="86"/>

</xml_diff>